<commit_message>
mise à jour temps tâche
</commit_message>
<xml_diff>
--- a/Audits/sommaireAudit3.xlsx
+++ b/Audits/sommaireAudit3.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Combaxe\Combaxe_Utilities\Audits\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9885"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -649,7 +644,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -659,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,7 +941,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>46</v>
@@ -1141,7 +1136,7 @@
       </c>
       <c r="E25" s="2">
         <f>SUM(E2:E22)</f>
-        <v>70.5</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>